<commit_message>
Added follow user feature to the implemenation
</commit_message>
<xml_diff>
--- a/RequirementsElicitation/RequirementsDB.xlsx
+++ b/RequirementsElicitation/RequirementsDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\hirehub\RequirementsElicitation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Hirehub\RequirementsElicitation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{956C53BB-CDBC-4ED7-8DD7-DFF9D59F9FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303FF9E1-8BE8-41B2-BC3E-9495F32F9F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1382,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="43" zoomScaleNormal="36" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="43" zoomScaleNormal="36" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added new diagrams to the repo and adjusted a few of them
</commit_message>
<xml_diff>
--- a/RequirementsElicitation/RequirementsDB.xlsx
+++ b/RequirementsElicitation/RequirementsDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wafia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wafia\Desktop\Hirehub\RequirementsElicitation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="352">
   <si>
     <t>REQ</t>
   </si>
@@ -325,30 +325,18 @@
     <t>FR-SK-002</t>
   </si>
   <si>
-    <t>FR-SK-003</t>
-  </si>
-  <si>
     <t>FR-SK-004</t>
   </si>
   <si>
     <t>Lock Screen During Assessment</t>
   </si>
   <si>
-    <t>Generate New Assessment After Cooldown</t>
-  </si>
-  <si>
     <t>When the user starts an assessment, the system shall lock the screen, preventing any navigation away from the assessment page. The user can only either complete the assessment or close the application, which will result in the submission of the current progress or failure.</t>
   </si>
   <si>
     <t>This ensures fairness by preventing users from switching apps or browsing for external help.</t>
   </si>
   <si>
-    <t>After the 24-hour cooldown period, the system shall generate a new, randomized assessment for the applicant if the job post is still available. The questions will be drawn from a randomized pool to ensure a different assessment is presented each time.</t>
-  </si>
-  <si>
-    <t>This ensures fairness by preventing applicants from reattempting the same questions and abusing the assessment process.</t>
-  </si>
-  <si>
     <t>FR-JM-005</t>
   </si>
   <si>
@@ -404,9 +392,6 @@
   </si>
   <si>
     <t>Employers can review candidates sorted by assessment and comparison scores, with options to shortlist or schedule interviews directly from the card.</t>
-  </si>
-  <si>
-    <t>FR-RM-011</t>
   </si>
   <si>
     <t>The system shall track whether the contract is signed and sent, and send reminders if necessary. It will also notify HR once the process is complete.</t>
@@ -512,30 +497,9 @@
     <t>FR-UM-019</t>
   </si>
   <si>
-    <t>Review Hiring Statistics</t>
-  </si>
-  <si>
-    <t>The system shall allow the CEO to review hiring statistics, including the number of applicants and successful hires.</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>FR-DASH-001</t>
-  </si>
-  <si>
-    <t>View System Analytics</t>
-  </si>
-  <si>
-    <t>FR-Admin-DASH-001</t>
-  </si>
-  <si>
     <t>AdminDashboard</t>
   </si>
   <si>
-    <t>The system shall allow SuperAdmin to view system-wide analytics, including total users, active users, and companies.</t>
-  </si>
-  <si>
     <t>Manage User Accounts</t>
   </si>
   <si>
@@ -549,21 +513,6 @@
   </si>
   <si>
     <t>The system shall allow SuperAdmin to manage user roles and permissions for CEOs, HR, and Job Seekers.</t>
-  </si>
-  <si>
-    <t>Monitor System Health</t>
-  </si>
-  <si>
-    <t>The system shall allow SuperAdmin to monitor the system's health, including server status, response times, and uptime.</t>
-  </si>
-  <si>
-    <t>View System Logs</t>
-  </si>
-  <si>
-    <t>FR-Admin-DASH-004</t>
-  </si>
-  <si>
-    <t>FR-Admin-DASH-005</t>
   </si>
   <si>
     <t>The system shall determine if the role is in-office or remote. For in-office roles, the system shall send an email asking the applicant to visit the company to sign the contract. For remote roles, the system shall send an email containing a link to an electronic contract, which the applicant must sign and return via email.</t>
@@ -1255,7 +1204,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1270,32 +1219,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1363,7 +1288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1387,9 +1312,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1424,22 +1346,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1451,20 +1370,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1473,38 +1392,38 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1786,21 +1705,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="136.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="53.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="255.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="255.77734375" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1850,10 +1769,10 @@
         <v>45</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -1876,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -1888,7 +1807,7 @@
         <v>48</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>48</v>
@@ -1900,7 +1819,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -1912,7 +1831,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>52</v>
@@ -1924,10 +1843,10 @@
         <v>45</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
@@ -1938,7 +1857,7 @@
         <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>55</v>
@@ -1950,10 +1869,10 @@
         <v>45</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="7" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -1990,7 +1909,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>61</v>
@@ -2002,10 +1921,10 @@
         <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
@@ -2013,13 +1932,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
@@ -2028,7 +1947,7 @@
         <v>45</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="H9" s="6"/>
     </row>
@@ -2052,7 +1971,7 @@
         <v>45</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>54</v>
@@ -2063,13 +1982,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>7</v>
@@ -2077,11 +1996,11 @@
       <c r="F11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="21" t="s">
-        <v>193</v>
+      <c r="G11" s="20" t="s">
+        <v>176</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
@@ -2089,13 +2008,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>7</v>
@@ -2103,8 +2022,8 @@
       <c r="F12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="21" t="s">
-        <v>196</v>
+      <c r="G12" s="20" t="s">
+        <v>179</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -2113,13 +2032,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>7</v>
@@ -2128,7 +2047,7 @@
         <v>45</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>57</v>
@@ -2139,13 +2058,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>14</v>
@@ -2154,7 +2073,7 @@
         <v>45</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>60</v>
@@ -2165,13 +2084,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>7</v>
@@ -2180,7 +2099,7 @@
         <v>45</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="H15" s="9"/>
     </row>
@@ -2189,13 +2108,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>14</v>
@@ -2204,10 +2123,10 @@
         <v>45</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2215,13 +2134,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>259</v>
+        <v>153</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>14</v>
@@ -2229,25 +2148,25 @@
       <c r="F17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="H17" s="15" t="s">
+      <c r="G17" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="20" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>260</v>
+        <v>154</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>243</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>7</v>
@@ -2255,25 +2174,25 @@
       <c r="F18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="20" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="G18" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>340</v>
+        <v>221</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>323</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
@@ -2281,23 +2200,23 @@
       <c r="F19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" s="20" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="G19" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>341</v>
+        <v>155</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>324</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>14</v>
@@ -2305,23 +2224,23 @@
       <c r="F20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="15" t="s">
-        <v>361</v>
-      </c>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" s="20" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="G20" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>263</v>
+        <v>222</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>246</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>14</v>
@@ -2329,25 +2248,25 @@
       <c r="F21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="20" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="G21" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>265</v>
+        <v>223</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>248</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>7</v>
@@ -2355,23 +2274,23 @@
       <c r="F22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="1:8" s="20" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="G22" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>270</v>
+        <v>224</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>253</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
@@ -2379,11 +2298,11 @@
       <c r="F23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>272</v>
+      <c r="G23" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
@@ -2391,13 +2310,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>7</v>
@@ -2406,7 +2325,7 @@
         <v>45</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H24" s="5"/>
     </row>
@@ -2415,13 +2334,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>7</v>
@@ -2430,7 +2349,7 @@
         <v>45</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="H25" s="5"/>
     </row>
@@ -2439,13 +2358,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>7</v>
@@ -2454,10 +2373,10 @@
         <v>45</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
@@ -2465,13 +2384,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>14</v>
@@ -2480,10 +2399,10 @@
         <v>45</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
@@ -2491,13 +2410,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>7</v>
@@ -2506,10 +2425,10 @@
         <v>45</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
@@ -2517,13 +2436,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>7</v>
@@ -2532,7 +2451,7 @@
         <v>45</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H29" s="5"/>
     </row>
@@ -2541,13 +2460,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>7</v>
@@ -2556,7 +2475,7 @@
         <v>45</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H30" s="5"/>
     </row>
@@ -2565,13 +2484,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>7</v>
@@ -2580,7 +2499,7 @@
         <v>45</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="H31" s="5"/>
     </row>
@@ -2589,13 +2508,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>7</v>
@@ -2604,7 +2523,7 @@
         <v>45</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="H32" s="5"/>
     </row>
@@ -2613,13 +2532,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>7</v>
@@ -2628,7 +2547,7 @@
         <v>45</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
       <c r="H33" s="5"/>
     </row>
@@ -2637,13 +2556,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>7</v>
@@ -2652,7 +2571,7 @@
         <v>45</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H34" s="5"/>
     </row>
@@ -2661,13 +2580,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>7</v>
@@ -2676,7 +2595,7 @@
         <v>45</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="H35" s="5"/>
     </row>
@@ -2685,13 +2604,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>7</v>
@@ -2700,7 +2619,7 @@
         <v>45</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
       <c r="H36" s="5"/>
     </row>
@@ -2709,13 +2628,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>7</v>
@@ -2724,7 +2643,7 @@
         <v>45</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="H37" s="5"/>
     </row>
@@ -2733,13 +2652,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>7</v>
@@ -2748,7 +2667,7 @@
         <v>45</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H38" s="5"/>
     </row>
@@ -2757,13 +2676,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>7</v>
@@ -2772,7 +2691,7 @@
         <v>45</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="H39" s="5"/>
     </row>
@@ -2781,13 +2700,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>7</v>
@@ -2796,7 +2715,7 @@
         <v>45</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="H40" s="5"/>
     </row>
@@ -2805,13 +2724,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>7</v>
@@ -2820,7 +2739,7 @@
         <v>45</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="H41" s="5"/>
     </row>
@@ -2829,13 +2748,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>7</v>
@@ -2844,7 +2763,7 @@
         <v>45</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H42" s="5"/>
     </row>
@@ -2853,13 +2772,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>7</v>
@@ -2868,7 +2787,7 @@
         <v>45</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
       <c r="H43" s="5"/>
     </row>
@@ -2880,7 +2799,7 @@
         <v>64</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>64</v>
@@ -2918,7 +2837,7 @@
         <v>65</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>70</v>
@@ -2932,7 +2851,7 @@
         <v>71</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>71</v>
@@ -2944,7 +2863,7 @@
         <v>65</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="H46" s="5"/>
     </row>
@@ -2953,13 +2872,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>14</v>
@@ -2968,7 +2887,7 @@
         <v>65</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="H47" s="5"/>
     </row>
@@ -2977,13 +2896,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>14</v>
@@ -2992,7 +2911,7 @@
         <v>65</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="H48" s="5"/>
     </row>
@@ -3001,13 +2920,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>14</v>
@@ -3016,10 +2935,10 @@
         <v>65</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.4">
@@ -3027,13 +2946,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>14</v>
@@ -3042,7 +2961,7 @@
         <v>65</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
       <c r="H50" s="5"/>
     </row>
@@ -3105,8 +3024,8 @@
       <c r="B53" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="16" t="s">
-        <v>208</v>
+      <c r="C53" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>81</v>
@@ -3117,8 +3036,8 @@
       <c r="F53" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G53" s="18" t="s">
-        <v>209</v>
+      <c r="G53" s="17" t="s">
+        <v>192</v>
       </c>
       <c r="H53" s="5"/>
     </row>
@@ -3130,7 +3049,7 @@
         <v>84</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>84</v>
@@ -3141,8 +3060,8 @@
       <c r="F54" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G54" s="18" t="s">
-        <v>366</v>
+      <c r="G54" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H54" s="5"/>
     </row>
@@ -3199,13 +3118,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>7</v>
@@ -3223,13 +3142,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>7</v>
@@ -3247,13 +3166,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>7</v>
@@ -3262,7 +3181,7 @@
         <v>74</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="H59" s="5"/>
     </row>
@@ -3271,13 +3190,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>14</v>
@@ -3286,7 +3205,7 @@
         <v>74</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="H60" s="5"/>
     </row>
@@ -3294,19 +3213,19 @@
       <c r="A61" s="3">
         <v>60</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E61" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="11" t="s">
+      <c r="E61" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G61" s="9" t="s">
@@ -3320,19 +3239,19 @@
       <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="D62" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E62" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="11" t="s">
+      <c r="E62" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="9" t="s">
@@ -3346,19 +3265,19 @@
       <c r="A63" s="3">
         <v>62</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E63" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F63" s="12" t="s">
+      <c r="E63" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="11" t="s">
         <v>8</v>
       </c>
       <c r="G63" s="9" t="s">
@@ -3372,25 +3291,25 @@
       <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="C64" s="14" t="s">
+      <c r="B64" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E64" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="13" t="s">
+      <c r="E64" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G64" s="15" t="s">
+      <c r="G64" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H64" s="15" t="s">
+      <c r="H64" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3398,51 +3317,51 @@
       <c r="A65" s="3">
         <v>64</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="D65" s="13" t="s">
+      <c r="C65" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E65" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F65" s="13" t="s">
+      <c r="E65" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="12" t="s">
         <v>8</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>276</v>
+        <v>258</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="3">
         <v>65</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D66" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E66" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F66" s="13" t="s">
+      <c r="E66" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G66" s="15" t="s">
+      <c r="G66" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H66" s="15" t="s">
+      <c r="H66" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3450,19 +3369,19 @@
       <c r="A67" s="3">
         <v>66</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="E67" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G67" s="9" t="s">
@@ -3476,19 +3395,19 @@
       <c r="A68" s="3">
         <v>67</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="D68" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E68" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="11" t="s">
+      <c r="E68" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G68" s="9" t="s">
@@ -3502,108 +3421,108 @@
       <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>296</v>
+      <c r="B69" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D69" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E69" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" s="11" t="s">
+      <c r="E69" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G69" s="9" t="s">
         <v>42</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3">
         <v>69</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D70" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D70" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E70" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F70" s="11" t="s">
+      <c r="E70" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G70" s="9" t="s">
         <v>22</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" s="3">
         <v>70</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="D71" s="11" t="s">
+      <c r="C71" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D71" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E71" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" s="11" t="s">
+      <c r="E71" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G71" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="H71" s="18" t="s">
-        <v>199</v>
+      <c r="G71" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="H71" s="17" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" s="3">
         <v>71</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="D72" s="11" t="s">
+      <c r="B72" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D72" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E72" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="11" t="s">
+      <c r="E72" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G72" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G72" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="13" t="s">
         <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
@@ -3625,70 +3544,70 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="22" t="s">
-        <v>101</v>
+      <c r="C74" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>98</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>97</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>74</v>
-      </c>
-      <c r="B75" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C75" s="10" t="s">
-        <v>102</v>
+      <c r="C75" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>99</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>346</v>
+        <v>7</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>97</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>75</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>100</v>
+        <v>76</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>7</v>
@@ -3697,24 +3616,24 @@
         <v>97</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>76</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>128</v>
+        <v>77</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>281</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>128</v>
+        <v>281</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>7</v>
@@ -3723,134 +3642,134 @@
         <v>97</v>
       </c>
       <c r="G77" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <v>78</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H78" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="H77" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3">
-        <v>77</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G78" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="H78" s="9" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>80</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F79" s="8" t="s">
+      <c r="D80" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>81</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G79" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="H79" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="3">
-        <v>79</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" s="8" t="s">
+      <c r="C81" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D81" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G80" s="9" t="s">
+      <c r="E81" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H81" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="H80" s="9" t="s">
+    </row>
+    <row r="82" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <v>82</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3">
-        <v>80</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="H81" s="9" t="s">
+      <c r="D82" s="8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3">
-        <v>81</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="E82" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G82" s="9" t="s">
         <v>120</v>
@@ -3859,393 +3778,279 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>123</v>
+        <v>282</v>
       </c>
       <c r="C83" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A84" s="3">
+        <v>84</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H84" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D83" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="H83" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3">
-        <v>83</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G84" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="H84" s="9"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" s="3">
-        <v>84</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>300</v>
+        <v>87</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>159</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E85" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E85" s="10" t="s">
         <v>7</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H85" s="9" t="s">
-        <v>127</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="H85" s="9"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A86" s="3">
-        <v>85</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="C86" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G86" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="D86" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="F86" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="G86" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="H86" s="9"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:8" ht="29.4" x14ac:dyDescent="0.65">
       <c r="A87" s="3">
-        <v>86</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C87" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="F87" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G87" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="H87" s="9"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+      <c r="B87" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="C87" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="D87" s="47" t="s">
+        <v>290</v>
+      </c>
+      <c r="E87" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="G87" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="H87" s="40"/>
+    </row>
+    <row r="88" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A88" s="3">
-        <v>87</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F88" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G88" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H88" s="9"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+        <v>92</v>
+      </c>
+      <c r="B88" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="C88" s="41" t="s">
+        <v>306</v>
+      </c>
+      <c r="D88" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="E88" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="G88" s="42" t="s">
+        <v>308</v>
+      </c>
+      <c r="H88" s="40"/>
+    </row>
+    <row r="89" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A89" s="3">
-        <v>88</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G89" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="H89" s="9"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+        <v>93</v>
+      </c>
+      <c r="B89" s="37" t="s">
+        <v>294</v>
+      </c>
+      <c r="C89" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="D89" s="47" t="s">
+        <v>295</v>
+      </c>
+      <c r="E89" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="G89" s="43" t="s">
+        <v>309</v>
+      </c>
+      <c r="H89" s="40"/>
+    </row>
+    <row r="90" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A90" s="3">
-        <v>89</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C90" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G90" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="H90" s="9"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+      <c r="B90" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="C90" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="D90" s="47" t="s">
+        <v>297</v>
+      </c>
+      <c r="E90" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G90" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="H90" s="40"/>
+    </row>
+    <row r="91" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A91" s="3">
-        <v>90</v>
-      </c>
-      <c r="B91" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C91" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E91" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H91" s="9"/>
-    </row>
-    <row r="92" spans="1:8" ht="29.4" x14ac:dyDescent="0.65">
+        <v>95</v>
+      </c>
+      <c r="B91" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="C91" s="37" t="s">
+        <v>313</v>
+      </c>
+      <c r="D91" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="E91" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="46" t="s">
+        <v>317</v>
+      </c>
+      <c r="G91" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="H91" s="7"/>
+    </row>
+    <row r="92" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A92" s="3">
-        <v>91</v>
-      </c>
-      <c r="B92" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="C92" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="C92" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="D92" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="E92" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="G92" s="45" t="s">
         <v>321</v>
       </c>
-      <c r="D92" s="42" t="s">
-        <v>307</v>
-      </c>
-      <c r="E92" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F92" s="43" t="s">
-        <v>310</v>
-      </c>
-      <c r="G92" s="44" t="s">
-        <v>322</v>
-      </c>
+      <c r="H92" s="40"/>
     </row>
     <row r="93" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A93" s="3">
-        <v>92</v>
-      </c>
-      <c r="B93" s="40" t="s">
-        <v>308</v>
-      </c>
-      <c r="C93" s="45" t="s">
-        <v>323</v>
-      </c>
-      <c r="D93" s="42" t="s">
-        <v>309</v>
-      </c>
-      <c r="E93" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F93" s="40" t="s">
-        <v>324</v>
-      </c>
-      <c r="G93" s="46" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A94" s="3">
-        <v>93</v>
-      </c>
-      <c r="B94" s="40" t="s">
-        <v>311</v>
-      </c>
-      <c r="C94" s="40" t="s">
-        <v>327</v>
-      </c>
-      <c r="D94" s="42" t="s">
-        <v>312</v>
-      </c>
-      <c r="E94" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F94" s="40" t="s">
-        <v>328</v>
-      </c>
-      <c r="G94" s="47" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A95" s="3">
-        <v>94</v>
-      </c>
-      <c r="B95" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="C95" s="48" t="s">
-        <v>329</v>
-      </c>
-      <c r="D95" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="E95" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F95" s="41" t="s">
-        <v>339</v>
-      </c>
-      <c r="G95" s="49" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A96" s="3">
-        <v>95</v>
-      </c>
-      <c r="B96" s="40" t="s">
-        <v>315</v>
-      </c>
-      <c r="C96" s="40" t="s">
-        <v>330</v>
-      </c>
-      <c r="D96" s="42" t="s">
-        <v>316</v>
-      </c>
-      <c r="E96" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F96" s="40" t="s">
-        <v>334</v>
-      </c>
-      <c r="G96" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A97" s="3">
-        <v>96</v>
-      </c>
-      <c r="B97" s="40" t="s">
-        <v>317</v>
-      </c>
-      <c r="C97" s="40" t="s">
-        <v>333</v>
-      </c>
-      <c r="D97" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="C93" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="E97" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F97" s="43" t="s">
-        <v>334</v>
-      </c>
-      <c r="G97" s="49" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A98" s="3">
-        <v>97</v>
-      </c>
-      <c r="B98" s="40" t="s">
+      <c r="D93" s="47" t="s">
+        <v>303</v>
+      </c>
+      <c r="E93" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93" s="46" t="s">
         <v>319</v>
       </c>
-      <c r="C98" s="40" t="s">
-        <v>335</v>
-      </c>
-      <c r="D98" s="42" t="s">
+      <c r="G93" s="39" t="s">
         <v>320</v>
       </c>
-      <c r="E98" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F98" s="40" t="s">
-        <v>336</v>
-      </c>
-      <c r="G98" s="44" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="F101" s="4"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="G102" s="2"/>
+      <c r="H93" s="40"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F96" s="4"/>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="G97" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4264,295 +4069,295 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="129.77734375" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="24" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="24"/>
+    <col min="1" max="1" width="12.21875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="129.77734375" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="22" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.2" x14ac:dyDescent="0.45">
-      <c r="A2" s="25" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="C3" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>301</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="F7" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>307</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>310</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>323</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>309</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>324</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>327</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>328</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>329</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>314</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>316</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>334</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="C7" s="36" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="C8" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>319</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>335</v>
-      </c>
-      <c r="C8" s="36" t="s">
+      <c r="F8" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>336</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>337</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-    </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="38"/>
-    </row>
-    <row r="11" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="38"/>
-    </row>
-    <row r="12" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="38"/>
-    </row>
-    <row r="13" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="38"/>
-    </row>
-    <row r="14" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="38"/>
-    </row>
-    <row r="15" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="38"/>
-    </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="38"/>
-    </row>
-    <row r="17" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="38"/>
-    </row>
-    <row r="18" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="38"/>
-    </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="38"/>
-    </row>
-    <row r="20" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="38"/>
-    </row>
-    <row r="21" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="38"/>
-    </row>
-    <row r="22" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="37"/>
-      <c r="G22" s="38"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="36"/>
+    </row>
+    <row r="11" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="36"/>
+    </row>
+    <row r="12" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="36"/>
+    </row>
+    <row r="13" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="36"/>
+    </row>
+    <row r="14" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="36"/>
+    </row>
+    <row r="15" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="36"/>
+    </row>
+    <row r="16" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="36"/>
+    </row>
+    <row r="17" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="36"/>
+    </row>
+    <row r="18" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="36"/>
+    </row>
+    <row r="19" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="36"/>
+    </row>
+    <row r="20" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="36"/>
+    </row>
+    <row r="21" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="36"/>
+    </row>
+    <row r="22" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="35"/>
+      <c r="G22" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fixed issues with front-end
</commit_message>
<xml_diff>
--- a/RequirementsElicitation/RequirementsDB.xlsx
+++ b/RequirementsElicitation/RequirementsDB.xlsx
@@ -1707,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24.6" x14ac:dyDescent="0.4"/>

</xml_diff>